<commit_message>
add auto scroll when report succes shown
</commit_message>
<xml_diff>
--- a/hasil/2024-06-04_monitoring_lama_perkara.xlsx
+++ b/hasil/2024-06-04_monitoring_lama_perkara.xlsx
@@ -704,7 +704,7 @@
         <v>12</v>
       </c>
       <c r="F7" s="10">
-        <v>94</v>
+        <v>99</v>
       </c>
       <c r="G7" s="10" t="s">
         <v>13</v>
@@ -750,7 +750,7 @@
         <v>12</v>
       </c>
       <c r="F9" s="10">
-        <v>93</v>
+        <v>98</v>
       </c>
       <c r="G9" s="10" t="s">
         <v>13</v>

</xml_diff>